<commit_message>
Update TDCASSCF data and its result Add/update Ishikawa's new simulated data
</commit_message>
<xml_diff>
--- a/Data/Global fitting.xlsx
+++ b/Data/Global fitting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Documents/FERMI 20144077 Ueda/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096D06B5-30EA-9140-AAF8-BCE79D6F0D47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F157CB-7915-2A4A-B160-C059E18AD930}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{20374876-1BA4-5248-8AA4-B248845CCD7C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" xr2:uid="{20374876-1BA4-5248-8AA4-B248845CCD7C}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="good3" sheetId="2" r:id="rId7"/>
     <sheet name="good4" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -88,9 +88,6 @@
     <t>beta4 (wonly)</t>
   </si>
   <si>
-    <t>Global-fitting (mixed)</t>
-  </si>
-  <si>
     <t>Parameters</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>beta4</t>
+  </si>
+  <si>
+    <t>Global-fitting (TDCASSCF)</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
       <calculatedColumnFormula>(0.044^2+0.029^2)^0.5</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{84B21B29-285C-1747-8894-D3E8281F3B23}" name="Global-fitting (TDHF)" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{3651E495-5C13-0D47-A136-72C60DEE199B}" name="Global-fitting (mixed)" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{3651E495-5C13-0D47-A136-72C60DEE199B}" name="Global-fitting (TDCASSCF)" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -413,13 +413,13 @@
     <tableColumn id="4" xr3:uid="{EB6B1E49-3619-BD4D-8504-14117BA9C375}" name="beta1 amp"/>
     <tableColumn id="3" xr3:uid="{54C3FCAB-1AB4-3243-A267-C4F36887055D}" name="beta1 shift" dataDxfId="44"/>
     <tableColumn id="10" xr3:uid="{441EE260-8A9E-714C-964C-331B3F50D12C}" name="beta1 shift error" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{55F5D209-0388-1B43-A1E6-AF47BB879B94}" name="beta2" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{6BDA6468-F14D-1945-89B3-D07DA4EDEFF2}" name="beta3 amp" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{74B9D932-3A08-EE4D-BFD3-D83A478C2213}" name="beta3 shift" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{9B42C196-5A31-C345-BEFF-4B6B192B1694}" name="beta3 shift error" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{1C91A754-6763-4743-905A-ECA0BA68D083}" name="beta4" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{B43AA49C-C7BE-5B4F-948F-761BA40EEFEF}" name="beta1m3 shift" dataDxfId="40"/>
-    <tableColumn id="14" xr3:uid="{05AC6EE6-B20F-884D-B287-7F52099EEDF0}" name="beta1m3 shift error" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{55F5D209-0388-1B43-A1E6-AF47BB879B94}" name="beta2" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{6BDA6468-F14D-1945-89B3-D07DA4EDEFF2}" name="beta3 amp" dataDxfId="41"/>
+    <tableColumn id="12" xr3:uid="{74B9D932-3A08-EE4D-BFD3-D83A478C2213}" name="beta3 shift" dataDxfId="40"/>
+    <tableColumn id="11" xr3:uid="{9B42C196-5A31-C345-BEFF-4B6B192B1694}" name="beta3 shift error" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{1C91A754-6763-4743-905A-ECA0BA68D083}" name="beta4" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{B43AA49C-C7BE-5B4F-948F-761BA40EEFEF}" name="beta1m3 shift" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{05AC6EE6-B20F-884D-B287-7F52099EEDF0}" name="beta1m3 shift error" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -431,14 +431,14 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{6623B9D1-76EF-FE48-8986-080FE9DEB127}" name="Dataset"/>
     <tableColumn id="2" xr3:uid="{6D19D5A1-75B9-C141-A90C-736658D05B85}" name="Photon (eV)"/>
-    <tableColumn id="15" xr3:uid="{7A17F56E-F457-2E42-BD4F-BFCA7F1AB58C}" name="beta1 amp" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{2F8F3D78-5300-474B-8251-146D751B8487}" name="beta1 shift" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{126954E7-0B32-0D48-BE43-B56594C7EDF8}" name="beta2" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{1869311F-4D11-AD44-ACBB-37A4D51372AE}" name="beta3 amp" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{301EBE7F-4C62-454D-BE9E-7006763666D6}" name="beta3 shift" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{A9183E8D-91F7-1942-A518-619EE60A25B9}" name="beta4" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{822AC06C-DB6A-CE4C-9D7C-3EB65607420D}" name="beta1m3 amp" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{E15E43D6-BBC5-5743-9C0A-1B33F3FE458A}" name="beta1m3 shift" dataDxfId="33"/>
+    <tableColumn id="15" xr3:uid="{7A17F56E-F457-2E42-BD4F-BFCA7F1AB58C}" name="beta1 amp" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{2F8F3D78-5300-474B-8251-146D751B8487}" name="beta1 shift" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{126954E7-0B32-0D48-BE43-B56594C7EDF8}" name="beta2" dataDxfId="33"/>
+    <tableColumn id="16" xr3:uid="{1869311F-4D11-AD44-ACBB-37A4D51372AE}" name="beta3 amp" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{301EBE7F-4C62-454D-BE9E-7006763666D6}" name="beta3 shift" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{A9183E8D-91F7-1942-A518-619EE60A25B9}" name="beta4" dataDxfId="30"/>
+    <tableColumn id="17" xr3:uid="{822AC06C-DB6A-CE4C-9D7C-3EB65607420D}" name="beta1m3 amp" dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{E15E43D6-BBC5-5743-9C0A-1B33F3FE458A}" name="beta1m3 shift" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -450,14 +450,14 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{260C2F96-5EEB-1040-BCF2-3F9DE679B72D}" name="Dataset"/>
     <tableColumn id="2" xr3:uid="{C4A7F33A-6285-914D-A3E0-8E6B54303316}" name="Photon (eV)"/>
-    <tableColumn id="15" xr3:uid="{F885CD15-3DA3-604C-B208-0B0292404995}" name="beta1 amp" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{500A4546-254C-FA4C-9C9B-1F503C7E21F7}" name="beta1 shift" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{A180CAE9-EC29-CC4A-82C6-7C6ED7295BBA}" name="beta2" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{42FFBAB4-D433-DF4D-B680-33447C1C1FA9}" name="beta3 amp" dataDxfId="30"/>
-    <tableColumn id="12" xr3:uid="{D84A7395-8776-E54B-AECB-76D98464A40F}" name="beta3 shift" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{ED7490B3-29BB-014D-BD10-61670799431D}" name="beta4" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{C77534EF-9A4C-804C-BA68-741FBE199533}" name="beta1m3 amp" dataDxfId="28"/>
-    <tableColumn id="13" xr3:uid="{92CC4E33-46A0-1E40-A49B-FFD5032FCBF8}" name="beta1m3 shift" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{F885CD15-3DA3-604C-B208-0B0292404995}" name="beta1 amp" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{500A4546-254C-FA4C-9C9B-1F503C7E21F7}" name="beta1 shift" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{A180CAE9-EC29-CC4A-82C6-7C6ED7295BBA}" name="beta2" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{42FFBAB4-D433-DF4D-B680-33447C1C1FA9}" name="beta3 amp" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{D84A7395-8776-E54B-AECB-76D98464A40F}" name="beta3 shift" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{ED7490B3-29BB-014D-BD10-61670799431D}" name="beta4" dataDxfId="22"/>
+    <tableColumn id="17" xr3:uid="{C77534EF-9A4C-804C-BA68-741FBE199533}" name="beta1m3 amp" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{92CC4E33-46A0-1E40-A49B-FFD5032FCBF8}" name="beta1m3 shift" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -468,13 +468,13 @@
   <autoFilter ref="A1:F9" xr:uid="{E75F0B0D-0D94-3E49-A820-FB59873CB593}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{247DAF93-E8E6-5242-B8FF-E9383571B89C}" name="Parameters"/>
-    <tableColumn id="2" xr3:uid="{4F0DCD9F-0E8E-4741-8ABF-97422FA0AB22}" name="Target (TDHF)" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{08B1E6DA-7404-4245-85DF-6815F398DCE3}" name="At first guess" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{ED1568B6-FE8F-9D44-918E-5FF4D0D57D79}" name="At first guess, diff" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{4F0DCD9F-0E8E-4741-8ABF-97422FA0AB22}" name="Target (TDHF)" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{08B1E6DA-7404-4245-85DF-6815F398DCE3}" name="At first guess" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{ED1568B6-FE8F-9D44-918E-5FF4D0D57D79}" name="At first guess, diff" dataDxfId="17">
       <calculatedColumnFormula>Table24[[#This Row],[Target (TDHF)]]-Table24[[#This Row],[At first guess]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E15A215C-CA39-2B41-8443-A31A28ED6C5B}" name="Optimized" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{50E84031-88AF-4845-B030-D7E1648F7CFB}" name="Optimized, diff" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{E15A215C-CA39-2B41-8443-A31A28ED6C5B}" name="Optimized" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{50E84031-88AF-4845-B030-D7E1648F7CFB}" name="Optimized, diff" dataDxfId="15">
       <calculatedColumnFormula>Table24[[#This Row],[Target (TDHF)]]-Table24[[#This Row],[Optimized]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -487,13 +487,13 @@
   <autoFilter ref="A1:F9" xr:uid="{97BB1FB8-A203-A54E-ACCF-BE6AA12A6A15}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1C3CDB8B-23FE-1646-849E-5C26C4E81AFA}" name="Parameters"/>
-    <tableColumn id="2" xr3:uid="{FE2507B2-B868-4040-BE2D-BFDD16AC2B86}" name="Target (TDHF)" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{19852F4E-EF53-8648-BA6B-0548C57A5C18}" name="At first guess" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{C3E07C66-A950-3147-9719-A9FDC2A5AFAD}" name="At first guess, diff" dataDxfId="19">
+    <tableColumn id="2" xr3:uid="{FE2507B2-B868-4040-BE2D-BFDD16AC2B86}" name="Target (TDHF)" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{19852F4E-EF53-8648-BA6B-0548C57A5C18}" name="At first guess" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{C3E07C66-A950-3147-9719-A9FDC2A5AFAD}" name="At first guess, diff" dataDxfId="12">
       <calculatedColumnFormula>Table245[[#This Row],[Target (TDHF)]]-Table245[[#This Row],[At first guess]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC11E292-0D5D-EB49-919D-CFC91DCEF9D9}" name="Optimized" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{E4DC6A3A-563C-8347-A139-4ADAC1DCD716}" name="Optimized, diff" dataDxfId="17">
+    <tableColumn id="4" xr3:uid="{FC11E292-0D5D-EB49-919D-CFC91DCEF9D9}" name="Optimized" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{E4DC6A3A-563C-8347-A139-4ADAC1DCD716}" name="Optimized, diff" dataDxfId="10">
       <calculatedColumnFormula>Table245[[#This Row],[Target (TDHF)]]-Table245[[#This Row],[Optimized]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -506,13 +506,13 @@
   <autoFilter ref="A1:F9" xr:uid="{9B806714-77E1-0E4C-A942-61A46D237004}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D1A4C508-CEFF-8C48-92B0-319416C4A1C7}" name="Parameters"/>
-    <tableColumn id="2" xr3:uid="{368694BC-C8D1-FA41-8146-D3F453CA7079}" name="Target (TDHF)" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{5BF0E5F1-690F-464B-AADE-F5BC6D1B8115}" name="At first guess" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{08EC8B0D-A54A-A84E-8164-7EA0E9FF66BB}" name="At first guess, diff" dataDxfId="14">
+    <tableColumn id="2" xr3:uid="{368694BC-C8D1-FA41-8146-D3F453CA7079}" name="Target (TDHF)" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{5BF0E5F1-690F-464B-AADE-F5BC6D1B8115}" name="At first guess" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{08EC8B0D-A54A-A84E-8164-7EA0E9FF66BB}" name="At first guess, diff" dataDxfId="7">
       <calculatedColumnFormula>Table2[[#This Row],[Target (TDHF)]]-Table2[[#This Row],[At first guess]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B6503BB4-B3CB-0541-B3D5-9FC40DFAD39C}" name="Optimized" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{63C9D9B3-E42B-5B4C-9C29-C753855419CA}" name="Optimized, diff" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{B6503BB4-B3CB-0541-B3D5-9FC40DFAD39C}" name="Optimized" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{63C9D9B3-E42B-5B4C-9C29-C753855419CA}" name="Optimized, diff" dataDxfId="5">
       <calculatedColumnFormula>Table2[[#This Row],[Target (TDHF)]]-Table2[[#This Row],[Optimized]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -525,13 +525,13 @@
   <autoFilter ref="A1:F9" xr:uid="{F2D9BC8D-D1A1-B648-9808-923D11AC4011}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{44135CAD-A952-A74F-A35D-FE793136BAF2}" name="Parameters"/>
-    <tableColumn id="2" xr3:uid="{7756D713-2051-8744-8B52-F8B9C4805067}" name="Target (TDHF)" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{82528208-E8CE-F74B-838C-3CEF9C1F41B3}" name="At first guess" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{A12B1083-511D-AD48-BE08-735B514C1EBA}" name="At first guess, diff" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{7756D713-2051-8744-8B52-F8B9C4805067}" name="Target (TDHF)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{82528208-E8CE-F74B-838C-3CEF9C1F41B3}" name="At first guess" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A12B1083-511D-AD48-BE08-735B514C1EBA}" name="At first guess, diff" dataDxfId="2">
       <calculatedColumnFormula>Table2456[[#This Row],[Target (TDHF)]]-Table2456[[#This Row],[At first guess]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A5EEA70D-6387-5B41-A475-BE2C2839FC9B}" name="Optimized" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{8558FAC4-2B5D-9E42-B7E9-B906CEE71874}" name="Optimized, diff" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{A5EEA70D-6387-5B41-A475-BE2C2839FC9B}" name="Optimized" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{8558FAC4-2B5D-9E42-B7E9-B906CEE71874}" name="Optimized, diff" dataDxfId="0">
       <calculatedColumnFormula>Table2456[[#This Row],[Target (TDHF)]]-Table2456[[#This Row],[Optimized]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -839,7 +839,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,7 +854,7 @@
     <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -865,13 +865,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -883,13 +883,13 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -913,7 +913,7 @@
       </c>
       <c r="F2" s="1">
         <f>TDCASSCF[[#This Row],[beta1 shift]]</f>
-        <v>1.4641090800000001</v>
+        <v>1.46432392</v>
       </c>
       <c r="G2" s="1">
         <v>1.2046150760000001</v>
@@ -931,8 +931,8 @@
         <v>1.0649999999999999</v>
       </c>
       <c r="K2" s="1">
-        <f>0--0.878</f>
-        <v>0.878</v>
+        <f>0--0.76</f>
+        <v>0.76</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -956,7 +956,7 @@
       </c>
       <c r="F3" s="1">
         <f>TDCASSCF[[#This Row],[beta1 shift]]</f>
-        <v>1.7039155699999999</v>
+        <v>1.7040937</v>
       </c>
       <c r="G3" s="1">
         <v>1.1620427879999999</v>
@@ -974,8 +974,8 @@
         <v>1.2090000000000001</v>
       </c>
       <c r="K3" s="1">
-        <f>0--1.084</f>
-        <v>1.0840000000000001</v>
+        <f>0--1.293</f>
+        <v>1.2929999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -999,7 +999,7 @@
       </c>
       <c r="F4" s="1">
         <f>TDCASSCF[[#This Row],[beta1 shift]]</f>
-        <v>1.44546716</v>
+        <v>1.4455554799999999</v>
       </c>
       <c r="G4" s="1">
         <v>1.265857813</v>
@@ -1017,8 +1017,8 @@
         <v>1.3859999999999999</v>
       </c>
       <c r="K4" s="1">
-        <f>0--1.284</f>
-        <v>1.284</v>
+        <f>0--0.484</f>
+        <v>0.48399999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="F5" s="1">
         <f>TDCASSCF[[#This Row],[beta1 shift]]</f>
-        <v>1.4626400100000001</v>
+        <v>1.46436035</v>
       </c>
       <c r="G5" s="1">
         <v>1.203680919</v>
@@ -1060,8 +1060,8 @@
         <v>1.0469999999999999</v>
       </c>
       <c r="K5" s="1">
-        <f>0--1.126</f>
-        <v>1.1259999999999999</v>
+        <f>0--0.763</f>
+        <v>0.76300000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1105,34 +1105,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1324,28 +1324,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1490,7 +1490,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1513,28 +1513,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1545,28 +1545,28 @@
         <v>15.9</v>
       </c>
       <c r="C2" s="1">
-        <v>0.67889792000000004</v>
+        <v>0.38327351999999998</v>
       </c>
       <c r="D2" s="1">
-        <v>1.4641090800000001</v>
+        <v>1.46432392</v>
       </c>
       <c r="E2" s="1">
-        <v>-0.14383199999999999</v>
+        <v>-0.325318</v>
       </c>
       <c r="F2" s="1">
-        <v>1.0939448899999999</v>
+        <v>0.61767013999999998</v>
       </c>
       <c r="G2" s="1">
-        <v>0.84018307000000003</v>
+        <v>0.84041102999999995</v>
       </c>
       <c r="H2" s="1">
-        <v>1.2764040000000001</v>
+        <v>1.6892309999999999</v>
       </c>
       <c r="I2" s="1">
-        <v>1.1598544399999999</v>
+        <v>0.65490848000000002</v>
       </c>
       <c r="J2" s="1">
-        <v>3.6327683899999998</v>
+        <v>3.6330639699999998</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1577,28 +1577,28 @@
         <v>14.3</v>
       </c>
       <c r="C3" s="1">
-        <v>0.53690568000000005</v>
+        <v>0.24744627999999999</v>
       </c>
       <c r="D3" s="1">
-        <v>1.7039155699999999</v>
+        <v>1.7040937</v>
       </c>
       <c r="E3" s="1">
-        <v>-0.52683000000000002</v>
+        <v>-0.66602499999999998</v>
       </c>
       <c r="F3" s="1">
-        <v>0.40808040000000001</v>
+        <v>0.18805526</v>
       </c>
       <c r="G3" s="1">
-        <v>8.0232510000000007E-2</v>
+        <v>8.0286999999999997E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>0.22451099999999999</v>
+        <v>0.27140799999999998</v>
       </c>
       <c r="I3" s="1">
-        <v>0.83528778999999997</v>
+        <v>0.38496394</v>
       </c>
       <c r="J3" s="1">
-        <v>2.5248769599999998</v>
+        <v>2.52493883</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1609,28 +1609,28 @@
         <v>19.100000000000001</v>
       </c>
       <c r="C4" s="1">
-        <v>1.19704126</v>
+        <v>0.73081366000000003</v>
       </c>
       <c r="D4" s="1">
-        <v>1.44546716</v>
+        <v>1.4455554799999999</v>
       </c>
       <c r="E4" s="1">
-        <v>0.66269299999999998</v>
+        <v>0.62240300000000004</v>
       </c>
       <c r="F4" s="1">
-        <v>0.83186950000000004</v>
+        <v>0.50780736000000004</v>
       </c>
       <c r="G4" s="1">
-        <v>0.63980868000000002</v>
+        <v>0.64041780000000004</v>
       </c>
       <c r="H4" s="1">
-        <v>0.36608600000000002</v>
+        <v>0.51112500000000005</v>
       </c>
       <c r="I4" s="1">
-        <v>0.95957194000000001</v>
+        <v>0.58543655999999999</v>
       </c>
       <c r="J4" s="1">
-        <v>2.6621207</v>
+        <v>2.6623596200000001</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1641,28 +1641,28 @@
         <v>15.9</v>
       </c>
       <c r="C5" s="1">
-        <v>0.75589994000000005</v>
+        <v>0.21347211999999999</v>
       </c>
       <c r="D5" s="1">
-        <v>1.4626400100000001</v>
+        <v>1.46436035</v>
       </c>
       <c r="E5" s="1">
-        <v>1.6507000000000001E-2</v>
+        <v>-0.36727199999999999</v>
       </c>
       <c r="F5" s="1">
-        <v>1.2161745500000001</v>
+        <v>0.34403180999999999</v>
       </c>
       <c r="G5" s="1">
-        <v>0.83920287000000005</v>
+        <v>0.84044969999999997</v>
       </c>
       <c r="H5" s="1">
-        <v>0.91537000000000002</v>
+        <v>1.7846759999999999</v>
       </c>
       <c r="I5" s="1">
-        <v>1.28849769</v>
+        <v>0.36477521000000002</v>
       </c>
       <c r="J5" s="1">
-        <v>3.63121406</v>
+        <v>3.6331141200000001</v>
       </c>
     </row>
   </sheetData>
@@ -1694,22 +1694,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1917,22 +1917,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2140,22 +2140,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2363,22 +2363,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>